<commit_message>
[ADD] DB Tables for skin_issues score_category user_info score_history & [ADD] API for skinIssues_list and scoreCategory_list
</commit_message>
<xml_diff>
--- a/Backend/DBDesign.xlsx
+++ b/Backend/DBDesign.xlsx
@@ -14,20 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>TABLE NAME</t>
   </si>
   <si>
+    <t>ATTRUBITE NAME</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
     <t>Skin Issues</t>
   </si>
   <si>
     <t>Id</t>
   </si>
   <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
     <t>IssueName</t>
   </si>
   <si>
+    <t>STRING</t>
+  </si>
+  <si>
     <t>IssueColor</t>
   </si>
   <si>
@@ -40,6 +52,9 @@
     <t>IsActive</t>
   </si>
   <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
     <t>Score Categories</t>
   </si>
   <si>
@@ -53,6 +68,24 @@
   </si>
   <si>
     <t>MaxScore</t>
+  </si>
+  <si>
+    <t>User Info</t>
+  </si>
+  <si>
+    <t>UserUuid</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Score History</t>
+  </si>
+  <si>
+    <t>Concerns</t>
+  </si>
+  <si>
+    <t>JSON</t>
   </si>
 </sst>
 </file>
@@ -668,9 +701,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -997,95 +1033,197 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="15.6363636363636" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1818181818182" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.63636363636364" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="1" t="s">
+    <row r="10" spans="2:3">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:3">
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
       <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="1" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>